<commit_message>
ATC classification, reduced argument number
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C00F10-835C-A64B-BED1-BFF156703007}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6BC78C-8CBB-B84A-84F9-F99B59329CE0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2760" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
     <sheet name="biomarkers" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -196,7 +196,7 @@
     <t>v20221017</t>
   </si>
   <si>
-    <t>23.03d</t>
+    <t>23.04d</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
removed generic words from drug aliases
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6BC78C-8CBB-B84A-84F9-F99B59329CE0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA41F6F3-0861-F946-A733-12DA4D9D9760}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2760" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="3660" yWindow="2760" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>url</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Freshour et al., Nucleic Acids Res, 2020; 33237278</t>
   </si>
   <si>
-    <t>Kim et al., Nucleic Acids Res, 2021; 33151290</t>
-  </si>
-  <si>
     <t>Ochoa et al., Nucleic Acids Res, 2021; 33196847</t>
   </si>
   <si>
@@ -166,24 +163,6 @@
     <t>v20200405</t>
   </si>
   <si>
-    <t>DepMap/PRISM</t>
-  </si>
-  <si>
-    <t>PRISM drug repurposing resource</t>
-  </si>
-  <si>
-    <t>Corsello et al., Nat cancer, 2020, 32613204</t>
-  </si>
-  <si>
-    <t>2019_Q4</t>
-  </si>
-  <si>
-    <t>prism_depmap</t>
-  </si>
-  <si>
-    <t>https://depmap.org/repurposing/</t>
-  </si>
-  <si>
     <t>Sioutos et al., J Biomed Inform, 2007; 16697710</t>
   </si>
   <si>
@@ -197,6 +176,12 @@
   </si>
   <si>
     <t>23.04d</t>
+  </si>
+  <si>
+    <t>v2023</t>
+  </si>
+  <si>
+    <t>Kim et al., Nucleic Acids Res, 2023; 36305812</t>
   </si>
 </sst>
 </file>
@@ -275,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -290,9 +275,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -612,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -656,10 +638,10 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -676,10 +658,10 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -716,7 +698,10 @@
         <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>25</v>
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
@@ -735,10 +720,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -776,93 +761,73 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
         <v>30</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
         <v>41</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
         <v>42</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
         <v>35</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -871,7 +836,6 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{3B961138-C221-624A-8638-558315D6A917}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{6F5ED4ED-DF8C-C64A-BE9A-5C3AC1C64E46}"/>
     <hyperlink ref="C4" r:id="rId4" xr:uid="{4FC7902F-19F5-A940-8A13-1E5B4757C830}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{CE340532-85B3-C549-9D74-6609E7F88FB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
NCI update + biomarker cleaning
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA41F6F3-0861-F946-A733-12DA4D9D9760}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731D9825-0623-6540-8D17-4B54D94623D4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2760" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="3660" yWindow="2760" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>url</t>
   </si>
@@ -139,30 +139,12 @@
     <t>Tamborero et al., Genome Med, 2018; 29592813</t>
   </si>
   <si>
-    <t>PMKB provides information about clinical interpretations of cancer variants in a structured way</t>
-  </si>
-  <si>
-    <t>Precision Medicine Knowledge Database</t>
-  </si>
-  <si>
     <t>Mitelman Database</t>
   </si>
   <si>
-    <t>https://pmkb.weill.cornell.edu/</t>
-  </si>
-  <si>
-    <t>Huang et al., J Am Med Inform Assoc, 2017; 27789569</t>
-  </si>
-  <si>
-    <t>pmkb</t>
-  </si>
-  <si>
     <t>Griffith et al., Nat Genet, 2017; 28138153</t>
   </si>
   <si>
-    <t>v20200405</t>
-  </si>
-  <si>
     <t>Sioutos et al., J Biomed Inform, 2007; 16697710</t>
   </si>
   <si>
@@ -175,13 +157,13 @@
     <t>v20221017</t>
   </si>
   <si>
-    <t>23.04d</t>
-  </si>
-  <si>
     <t>v2023</t>
   </si>
   <si>
     <t>Kim et al., Nucleic Acids Res, 2023; 36305812</t>
+  </si>
+  <si>
+    <t>23.05e</t>
   </si>
 </sst>
 </file>
@@ -594,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -641,7 +623,7 @@
         <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -658,10 +640,10 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
         <v>45</v>
-      </c>
-      <c r="E3" t="s">
-        <v>49</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -698,10 +680,10 @@
         <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
@@ -720,10 +702,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -767,7 +749,7 @@
         <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
         <v>31</v>
@@ -775,7 +757,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>26</v>
@@ -784,7 +766,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
         <v>30</v>
@@ -792,41 +774,21 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
+        <v>33</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -834,8 +796,7 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{C0E82506-6BF0-3F41-934A-7D3FE7BB11BC}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{3B961138-C221-624A-8638-558315D6A917}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{6F5ED4ED-DF8C-C64A-BE9A-5C3AC1C64E46}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{4FC7902F-19F5-A940-8A13-1E5B4757C830}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{6F5ED4ED-DF8C-C64A-BE9A-5C3AC1C64E46}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
NCI/OTP update june 2023
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731D9825-0623-6540-8D17-4B54D94623D4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8F883A-13B5-874F-946A-8409C2CFB822}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2760" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="3660" yWindow="2760" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
@@ -151,9 +151,6 @@
     <t>v20230119</t>
   </si>
   <si>
-    <t>2023.02</t>
-  </si>
-  <si>
     <t>v20221017</t>
   </si>
   <si>
@@ -163,7 +160,10 @@
     <t>Kim et al., Nucleic Acids Res, 2023; 36305812</t>
   </si>
   <si>
-    <t>23.05e</t>
+    <t>23.06d</t>
+  </si>
+  <si>
+    <t>2023.06</t>
   </si>
 </sst>
 </file>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -623,7 +623,7 @@
         <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -643,7 +643,7 @@
         <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -680,10 +680,10 @@
         <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
@@ -704,7 +704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -786,7 +786,7 @@
         <v>36</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
NCI/OTP and CIViC update - Oct 2023
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CCA0D8-F1E9-D343-9A6C-6FB45D1EFE84}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34105FF4-7FED-C944-9D30-4EAB5C0A5894}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="3700" windowWidth="33580" windowHeight="16980" activeTab="1" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="2260" yWindow="3700" windowWidth="33580" windowHeight="16980" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
@@ -142,9 +142,6 @@
     <t>Kim et al., Nucleic Acids Res, 2023; 36305812</t>
   </si>
   <si>
-    <t>2023.06</t>
-  </si>
-  <si>
     <t>source_description</t>
   </si>
   <si>
@@ -193,10 +190,13 @@
     <t>https://www.dgidb.org/faq</t>
   </si>
   <si>
-    <t>23.08d</t>
-  </si>
-  <si>
     <t>v20230803</t>
+  </si>
+  <si>
+    <t>23.09d</t>
+  </si>
+  <si>
+    <t>2023.09</t>
   </si>
 </sst>
 </file>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -632,25 +632,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -667,16 +667,16 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -699,10 +699,10 @@
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -725,10 +725,10 @@
         <v>13</v>
       </c>
       <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -751,10 +751,10 @@
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I5" s="3"/>
     </row>
@@ -777,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -798,25 +798,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -837,10 +837,10 @@
         <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -854,16 +854,16 @@
         <v>24</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -886,10 +886,10 @@
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OTP 2023.12, Mitelmandb 2023-10
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34105FF4-7FED-C944-9D30-4EAB5C0A5894}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098185D6-BCDD-D44B-A83D-9AEF05E354CB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="3700" windowWidth="33580" windowHeight="16980" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="8860" yWindow="8400" windowWidth="33580" windowHeight="16980" activeTab="1" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
@@ -190,13 +190,13 @@
     <t>https://www.dgidb.org/faq</t>
   </si>
   <si>
-    <t>v20230803</t>
-  </si>
-  <si>
     <t>23.09d</t>
   </si>
   <si>
-    <t>2023.09</t>
+    <t>2023.12</t>
+  </si>
+  <si>
+    <t>v20231016</t>
   </si>
 </sst>
 </file>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -667,7 +667,7 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -693,7 +693,7 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -777,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -854,7 +854,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
CIVIC, NCI Thesaurus, MitelmanDB and Depmap update
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F19DD95-54C8-914C-9CDB-A112510C8E31}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D0E812-F58C-1C45-9682-835B290A2C58}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="2880" windowWidth="33580" windowHeight="16980" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="2260" yWindow="500" windowWidth="33580" windowHeight="16980" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>source</t>
   </si>
@@ -136,9 +136,6 @@
     <t>v20221017</t>
   </si>
   <si>
-    <t>v2023</t>
-  </si>
-  <si>
     <t>Kim et al., Nucleic Acids Res, 2023; 36305812</t>
   </si>
   <si>
@@ -190,13 +187,37 @@
     <t>https://www.dgidb.org/faq</t>
   </si>
   <si>
-    <t>v20240415</t>
-  </si>
-  <si>
-    <t>24.05d</t>
-  </si>
-  <si>
     <t>2024.06</t>
+  </si>
+  <si>
+    <t>v20240715</t>
+  </si>
+  <si>
+    <t>v2024</t>
+  </si>
+  <si>
+    <t>depmap</t>
+  </si>
+  <si>
+    <t>https://depmap.org</t>
+  </si>
+  <si>
+    <t>Tsherniak et al., Cell, 2017; 28753430</t>
+  </si>
+  <si>
+    <t>24Q2</t>
+  </si>
+  <si>
+    <t>https://depmap.org/portal/data_page/?tab=overview</t>
+  </si>
+  <si>
+    <t>DepMap</t>
+  </si>
+  <si>
+    <t>The Cancer Dependency Map</t>
+  </si>
+  <si>
+    <t>24.07e</t>
   </si>
 </sst>
 </file>
@@ -613,7 +634,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -632,25 +653,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -667,16 +688,16 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -693,16 +714,16 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -725,10 +746,10 @@
         <v>13</v>
       </c>
       <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -742,19 +763,19 @@
         <v>17</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I5" s="3"/>
     </row>
@@ -775,10 +796,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -798,25 +819,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -837,10 +858,10 @@
         <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -860,10 +881,10 @@
         <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -886,10 +907,36 @@
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NCI 24.09e, OTP 2024.09, skip DGIDB chembl map
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D0E812-F58C-1C45-9682-835B290A2C58}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C444E5F-BB46-F646-8A83-3B244929DCDA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="500" windowWidth="33580" windowHeight="16980" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="2260" yWindow="500" windowWidth="33580" windowHeight="16980" activeTab="1" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
@@ -187,12 +187,6 @@
     <t>https://www.dgidb.org/faq</t>
   </si>
   <si>
-    <t>2024.06</t>
-  </si>
-  <si>
-    <t>v20240715</t>
-  </si>
-  <si>
     <t>v2024</t>
   </si>
   <si>
@@ -217,7 +211,13 @@
     <t>The Cancer Dependency Map</t>
   </si>
   <si>
-    <t>24.07e</t>
+    <t>2024.09</t>
+  </si>
+  <si>
+    <t>24.09e</t>
+  </si>
+  <si>
+    <t>v20241015</t>
   </si>
 </sst>
 </file>
@@ -633,7 +633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -688,7 +688,7 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -714,7 +714,7 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -766,7 +766,7 @@
         <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
         <v>18</v>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -875,7 +875,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>25</v>
@@ -915,28 +915,28 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
         <v>57</v>
       </c>
-      <c r="D5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" t="s">
-        <v>59</v>
-      </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
         <v>51</v>
       </c>
       <c r="H5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NCI 24.10d & CIVIC 20241108
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C444E5F-BB46-F646-8A83-3B244929DCDA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE805809-BAD4-4A45-8BF2-9418CD2DBD75}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="500" windowWidth="33580" windowHeight="16980" activeTab="1" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="2240" yWindow="500" windowWidth="45200" windowHeight="19820" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
@@ -214,10 +214,10 @@
     <t>2024.09</t>
   </si>
   <si>
-    <t>24.09e</t>
-  </si>
-  <si>
     <t>v20241015</t>
+  </si>
+  <si>
+    <t>24.10d</t>
   </si>
 </sst>
 </file>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -714,7 +714,7 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -798,7 +798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -875,7 +875,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
civic update and fusion alias filtering
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A99D66-B18B-6442-B188-F6C607F680EA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC78865-67D4-9E47-A21C-EE069EB2B53D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19820" activeTab="1" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19820" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
@@ -193,10 +193,10 @@
     <t>v20241015</t>
   </si>
   <si>
-    <t>24.11d</t>
-  </si>
-  <si>
     <t>24Q4</t>
+  </si>
+  <si>
+    <t>24.12e</t>
   </si>
 </sst>
 </file>
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -691,7 +691,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -747,7 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -876,7 +876,7 @@
         <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
updates to CIViC and MitelmanDB
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC78865-67D4-9E47-A21C-EE069EB2B53D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69847C5D-8477-944B-BAE1-F883E5E2644A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19820" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19820" activeTab="1" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
     <sheet name="biomarkers" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateCount="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -190,13 +190,13 @@
     <t>2024.09</t>
   </si>
   <si>
-    <t>v20241015</t>
-  </si>
-  <si>
     <t>24Q4</t>
   </si>
   <si>
     <t>24.12e</t>
+  </si>
+  <si>
+    <t>v20250115</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -691,7 +691,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -824,7 +824,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>19</v>
@@ -876,7 +876,7 @@
         <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
civic update and NCI thesaurus update
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69EB1CF-8EA9-1149-A28A-BAB9320340C4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23968A10-B463-CB41-9071-3CF9AFA17554}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19820" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -196,7 +196,7 @@
     <t>v20250115</t>
   </si>
   <si>
-    <t>25.01d</t>
+    <t>25.02d</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
NCI Thesaurus, Mitelmandb update - aug 2025
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34D9230-63BD-1649-817E-0B0DF577664C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1527F8E7-759B-C744-8E68-7AC8ACA4EE7A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19820" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -187,16 +187,16 @@
     <t>The Cancer Dependency Map</t>
   </si>
   <si>
-    <t>v20250410</t>
-  </si>
-  <si>
     <t>2025.06</t>
   </si>
   <si>
     <t>25Q2</t>
   </si>
   <si>
-    <t>25.05d</t>
+    <t>25.07d</t>
+  </si>
+  <si>
+    <t>v20250710</t>
   </si>
 </sst>
 </file>
@@ -665,7 +665,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -691,7 +691,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -748,7 +748,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -824,7 +824,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>19</v>
@@ -876,7 +876,7 @@
         <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
NCI thesaurus and CIViC update
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1527F8E7-759B-C744-8E68-7AC8ACA4EE7A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33F83AE-33DD-EF48-8B15-28AD8C6D4D37}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19820" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -193,10 +193,10 @@
     <t>25Q2</t>
   </si>
   <si>
-    <t>25.07d</t>
-  </si>
-  <si>
     <t>v20250710</t>
+  </si>
+  <si>
+    <t>25.08d</t>
   </si>
 </sst>
 </file>
@@ -691,7 +691,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -824,7 +824,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
fix DepMap and Mitelmandb datestamp, update CIViC
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B4B6C5-8FA6-B04E-9DD3-C910B2FF8591}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0B39CB-19D5-104C-873F-BFDA052D9C2F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19820" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -166,9 +166,6 @@
     <t>Free/open access</t>
   </si>
   <si>
-    <t>v2024</t>
-  </si>
-  <si>
     <t>depmap</t>
   </si>
   <si>
@@ -187,9 +184,6 @@
     <t>The Cancer Dependency Map</t>
   </si>
   <si>
-    <t>25Q2</t>
-  </si>
-  <si>
     <t>v20250710</t>
   </si>
   <si>
@@ -197,6 +191,12 @@
   </si>
   <si>
     <t>2025.09</t>
+  </si>
+  <si>
+    <t>25Q3</t>
+  </si>
+  <si>
+    <t>v2025</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -665,7 +665,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -691,7 +691,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -717,7 +717,7 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -748,7 +748,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -824,7 +824,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>19</v>
@@ -864,28 +864,28 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
         <v>51</v>
       </c>
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
       <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
         <v>48</v>
       </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5" t="s">
         <v>45</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Mitelmandb sites, NCI Thesaurus 25.09e
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0B39CB-19D5-104C-873F-BFDA052D9C2F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D657EEE-C4A9-084B-A7F1-3E2C2D367BD2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19820" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -187,9 +187,6 @@
     <t>v20250710</t>
   </si>
   <si>
-    <t>25.08d</t>
-  </si>
-  <si>
     <t>2025.09</t>
   </si>
   <si>
@@ -197,6 +194,9 @@
   </si>
   <si>
     <t>v2025</t>
+  </si>
+  <si>
+    <t>25.09e</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -665,7 +665,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -691,7 +691,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -717,7 +717,7 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -876,7 +876,7 @@
         <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
update Mitelmandb and CIViC
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D657EEE-C4A9-084B-A7F1-3E2C2D367BD2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB095E2-4ABB-914A-AA4E-A60BCA8BD197}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19820" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19820" activeTab="1" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
@@ -184,9 +184,6 @@
     <t>The Cancer Dependency Map</t>
   </si>
   <si>
-    <t>v20250710</t>
-  </si>
-  <si>
     <t>2025.09</t>
   </si>
   <si>
@@ -197,6 +194,9 @@
   </si>
   <si>
     <t>25.09e</t>
+  </si>
+  <si>
+    <t>v20250815</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -665,7 +665,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -691,7 +691,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -717,7 +717,7 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -824,7 +824,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>19</v>
@@ -876,7 +876,7 @@
         <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
NCI thesaurus + CIViC update
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAFCC22-ED0F-4E44-BDA5-DF79A5A3252F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1798C4C-1E38-F24E-92DD-A8B9FDFE500E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="1360" windowWidth="35840" windowHeight="19820" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="35840" windowHeight="19820" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
@@ -196,7 +196,7 @@
     <t>v20250815</t>
   </si>
   <si>
-    <t>25.10d</t>
+    <t>25.11d</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
civic update + NCI thesaurus 26.01d
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharm_oncox.xlsx
+++ b/data-raw/metadata_pharm_oncox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/packages/package__pharmOncoX/pharmOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335ABEC8-E339-5341-9194-C5BC829EF263}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BB0252-63AC-184E-9D04-A9CE4C61F467}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="35840" windowHeight="19820" activeTab="1" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="35840" windowHeight="19820" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
@@ -193,10 +193,10 @@
     <t>2025.12</t>
   </si>
   <si>
-    <t>25.12e</t>
-  </si>
-  <si>
     <t>v20260115</t>
+  </si>
+  <si>
+    <t>26.01d</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -691,7 +691,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932642DA-7C44-1E43-949C-73113CAEBEC0}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -824,7 +824,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>19</v>

</xml_diff>